<commit_message>
Completed BVA Updates to match the new shared dea changes
</commit_message>
<xml_diff>
--- a/uploads/excel/sof_template.xlsx
+++ b/uploads/excel/sof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NKarisa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFB0AB4-605E-4AE6-9F69-467899C35620}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2278A49B-7D09-4BEB-A147-1643D1DE0EE9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12770" windowHeight="3540" xr2:uid="{DFD839DC-7D29-4632-9F74-6705A52DA9F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>sof_code</t>
   </si>
@@ -54,19 +54,25 @@
     <t>budget_section</t>
   </si>
   <si>
-    <t>Test SOF 1</t>
-  </si>
-  <si>
-    <t>Test DEA 3</t>
-  </si>
-  <si>
-    <t>Test DEA 4</t>
-  </si>
-  <si>
     <t>72818;72809;72802;72800</t>
   </si>
   <si>
     <t>72815;72816</t>
+  </si>
+  <si>
+    <t>Test SOF 2</t>
+  </si>
+  <si>
+    <t>Test SOF 3</t>
+  </si>
+  <si>
+    <t>Test DEA 5</t>
+  </si>
+  <si>
+    <t>Test DEA 6</t>
+  </si>
+  <si>
+    <t>Test DEA 7</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,10 +476,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1234567</v>
+        <v>823234</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>43466</v>
@@ -482,16 +488,16 @@
         <v>43830</v>
       </c>
       <c r="E2">
-        <v>76543</v>
+        <v>88890</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -499,10 +505,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1234567</v>
+        <v>823234</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>43466</v>
@@ -511,10 +517,10 @@
         <v>43830</v>
       </c>
       <c r="E3">
-        <v>87654</v>
+        <v>76542</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -528,10 +534,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>1234567</v>
+        <v>765865</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>43466</v>
@@ -540,16 +546,16 @@
         <v>43830</v>
       </c>
       <c r="E4">
-        <v>98765</v>
+        <v>87569</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I4">
         <v>0</v>

</xml_diff>